<commit_message>
add filter; fix bug realisasi, import data kepegawaian, laporan jam realisasi
</commit_message>
<xml_diff>
--- a/public/document/data-kepegawaian-inspektorat-utama.xlsx
+++ b/public/document/data-kepegawaian-inspektorat-utama.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\skripsi\simwas-app\public\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2293E52-DCAC-400E-A75C-CF0EFED4A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E17E044-3BE0-4F12-A37F-AD702FAD91FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DAC557F2-CDDA-4199-A856-A37BC1992612}"/>
   </bookViews>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>nip</t>
   </si>
   <si>
-    <t>jenis_data_kepegawaian</t>
-  </si>
-  <si>
     <t>nilai</t>
   </si>
   <si>
@@ -45,6 +42,12 @@
   </si>
   <si>
     <t>Nama Pegawai</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ID_jenis_data_kepegawaian</t>
   </si>
 </sst>
 </file>
@@ -419,24 +422,24 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="25.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -460,10 +463,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -473,20 +476,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8464EE1-0117-41C1-B6D3-A124C6C0C97D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>